<commit_message>
check the all code
</commit_message>
<xml_diff>
--- a/FinalResults/trajectoryOpt.xlsx
+++ b/FinalResults/trajectoryOpt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koray_0\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833342D9-B03D-4B09-88AD-E7DE1055E0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57776F1-11AA-4293-A522-6C815A37D970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="15" windowWidth="20730" windowHeight="11040" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
   </bookViews>
@@ -505,12 +505,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -525,6 +519,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,41 +862,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE33DE-026B-47FC-A290-185B7A79B5AD}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="30.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="30.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="17.375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="17.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.7109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="12" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.125" style="1"/>
+    <col min="19" max="19" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -936,7 +936,7 @@
       <c r="M2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="11" t="s">
         <v>109</v>
       </c>
       <c r="O2" s="2" t="s">
@@ -958,8 +958,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1004,8 +1004,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1048,8 +1048,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1092,29 +1092,29 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-    </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1213,28 +1213,28 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-    </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1351,28 +1351,28 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-    </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -1394,14 +1394,14 @@
       <c r="J15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="L15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
       <c r="O15" s="1">
         <v>1.9799999999999999E-4</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>0.13206999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1428,14 +1428,14 @@
       <c r="F16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
       <c r="O16" s="1">
         <v>9.1100000000000003E-4</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>6.5002000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1462,14 +1462,14 @@
       <c r="F17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="L17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
       <c r="O17" s="1">
         <v>1.3799999999999999E-3</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>0.13918</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>70</v>
       </c>
@@ -1499,14 +1499,14 @@
       <c r="F18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
       <c r="O18" s="1">
         <v>8.9630000000000005E-3</v>
       </c>
@@ -1520,28 +1520,28 @@
         <v>8.3160000000000005E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-    </row>
-    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1563,14 +1563,14 @@
       <c r="H20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
       <c r="O20" s="1">
         <v>2.0690000000000001E-3</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>2.1878999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>75</v>
       </c>
@@ -1600,14 +1600,14 @@
       <c r="H21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="L21" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
       <c r="O21" s="1">
         <v>1.3270000000000001E-3</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>1.0095E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>76</v>
       </c>
@@ -1637,14 +1637,14 @@
       <c r="H22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="L22" s="11" t="s">
+      <c r="L22" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
       <c r="O22" s="1">
         <v>1.0020000000000001E-3</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>5.6469999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
@@ -1677,14 +1677,14 @@
       <c r="H23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L23" s="11" t="s">
+      <c r="L23" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
       <c r="O23" s="1">
         <v>8.3500000000000002E-4</v>
       </c>
@@ -1698,28 +1698,28 @@
         <v>1.0437999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-    </row>
-    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>101</v>
       </c>
@@ -1763,17 +1763,20 @@
         <v>4.6030000000000003E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="C26" s="1">
+        <v>2.9904999999999999</v>
+      </c>
+      <c r="K26" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L26" s="11" t="s">
+      <c r="L26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="M26" s="11" t="s">
+      <c r="M26" s="9" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
keep going data 18
</commit_message>
<xml_diff>
--- a/FinalResults/trajectoryOpt.xlsx
+++ b/FinalResults/trajectoryOpt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koray\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC66A27E-08E7-423D-A2E5-7B3A2CB6E723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5208067-418C-4F25-A745-2AAEA91B8BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="122">
   <si>
     <t>Single Target - Single Section</t>
   </si>
@@ -126,24 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">  0 | 0.03 | 0.03</t>
-  </si>
-  <si>
-    <t>2.3901      1.6771      1.4802</t>
-  </si>
-  <si>
-    <t>0.75497      0.6752     0.60732</t>
-  </si>
-  <si>
-    <t>0.7541392     0.5660859     0.7463692</t>
-  </si>
-  <si>
-    <t>10.12181      11.57644      3.232965</t>
-  </si>
-  <si>
-    <t>50.92372      41.07672       52.2669</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 99.96      132.6114      81.72722</t>
   </si>
   <si>
     <r>
@@ -160,66 +142,15 @@
     </r>
   </si>
   <si>
-    <t>0.7636308     0.6928579     0.6575524</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.87688      7.512444      17.27889 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">51.05659      45.13527      66.79552 </t>
-  </si>
-  <si>
-    <t>133.1323      113.7784      106.1036</t>
-  </si>
-  <si>
-    <t>0.7558156     0.6254563     0.6632029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.29754      17.82162       16.7607 </t>
-  </si>
-  <si>
-    <t>57.79255      45.02585      48.71717</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 104.5205      135.4288       119.958</t>
-  </si>
-  <si>
     <t xml:space="preserve">Single Target Single  Section </t>
   </si>
   <si>
     <t>100 1 0.1 (Target End Time)</t>
   </si>
   <si>
-    <t xml:space="preserve">   5.06209      13.6765      1.89744</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8.93817      4.34307      11.3192</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4.6377      6.3734      5.5057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     2.2492      3.2283     0.86181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.85125     0.53054     0.52452 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.50211     0.71177     0.94338  </t>
-  </si>
-  <si>
-    <t>4.2593      2.1089      5.4893</t>
-  </si>
-  <si>
     <t>Line_DoubleTarget_NoKpKd_SingleSection</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.752055     0.892478     0.695824 </t>
-  </si>
-  <si>
-    <t>4.26988      16.7613      8.25976</t>
-  </si>
-  <si>
     <t>0, 0.02, 0.01</t>
   </si>
   <si>
@@ -241,18 +172,6 @@
     <t>0, 0.03, 0.04</t>
   </si>
   <si>
-    <t>0.57893     0.56809      0.8867</t>
-  </si>
-  <si>
-    <t>2.4998      5.1495      8.4775</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.852806     0.890479      0.96536 </t>
-  </si>
-  <si>
-    <t>8.38298      12.4055      11.3756</t>
-  </si>
-  <si>
     <t>0, 0.02, 0.02</t>
   </si>
   <si>
@@ -262,12 +181,6 @@
     <t>failed</t>
   </si>
   <si>
-    <t>0.50081     0.96823     0.50002</t>
-  </si>
-  <si>
-    <t>6.2503      2.8003      1.8142</t>
-  </si>
-  <si>
     <t>0, 0.03, 0.045</t>
   </si>
   <si>
@@ -289,18 +202,6 @@
     <t>zeta2</t>
   </si>
   <si>
-    <t>1.81      2.2238      4.6611</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2.5805       1.067     0.61792</t>
-  </si>
-  <si>
-    <t>2.5805     0.66763      7.9999</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2.5805     0.51611      4.5722</t>
-  </si>
-  <si>
     <t>w3</t>
   </si>
   <si>
@@ -410,13 +311,115 @@
   </si>
   <si>
     <t>data20</t>
+  </si>
+  <si>
+    <t>14.9847           15      3.01046</t>
+  </si>
+  <si>
+    <t>7.84644      4.58378      12.9908</t>
+  </si>
+  <si>
+    <t>3.2827        6.95      6.0672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.751498     0.676485     0.878121 </t>
+  </si>
+  <si>
+    <t>13.0375      14.9529      3.58575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.74946     0.79341     0.82094 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6.846      2.8914      7.0493</t>
+  </si>
+  <si>
+    <t>0.9958    0.6091    0.8745</t>
+  </si>
+  <si>
+    <t>11.9855    4.2149    4.5718</t>
+  </si>
+  <si>
+    <t>0.75196     0.564448     0.960431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.84823      18.5548      5.14193 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 60.5674      60.4803      59.9803</t>
+  </si>
+  <si>
+    <t>89.6256      88.6417      91.7912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9160724     0.8638073     0.5727551  </t>
+  </si>
+  <si>
+    <t>10.69823      3.682638      7.553252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53.38334      40.00147      51.29529 </t>
+  </si>
+  <si>
+    <t>96.4811      92.42004      107.2134</t>
+  </si>
+  <si>
+    <t>0.7378902     0.7642485     0.7004045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.6893       15.8735      13.69968 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">59.56614      66.37721      46.04473 </t>
+  </si>
+  <si>
+    <t>108.7981      131.4733      94.46455</t>
+  </si>
+  <si>
+    <t>0, 0.025, 0.045</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.727287     0.730442     0.721689 </t>
+  </si>
+  <si>
+    <t>6.1908      8.55466      15.6824</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.74941      0.82108     0.733546  </t>
+  </si>
+  <si>
+    <t>7.5277      16.5885      8.62631</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.73358     0.83923     0.78457</t>
+  </si>
+  <si>
+    <t>0.10025      2.8951      2.4026</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.75529           1      0.5876</t>
+  </si>
+  <si>
+    <t>1.066      2.1154      1.3248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.45319      1.3363      2.8087 </t>
+  </si>
+  <si>
+    <t>5.0797      2.8558      1.5681</t>
+  </si>
+  <si>
+    <t>5.0797      1.6178      6.7134</t>
+  </si>
+  <si>
+    <t>5.0797      5.2114      4.2905</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -875,10 +878,10 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.25" style="1" bestFit="1" customWidth="1"/>
@@ -898,7 +901,7 @@
     <col min="21" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
@@ -909,7 +912,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:20" ht="15">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -920,19 +923,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>4</v>
@@ -941,25 +944,25 @@
         <v>5</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>13</v>
@@ -971,7 +974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -979,14 +982,14 @@
         <v>9</v>
       </c>
       <c r="C3" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1014,23 +1017,23 @@
         <v>6.8770999999999999E-2</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4">
-        <v>2.9703499999999998</v>
+        <v>1.8973</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -1058,23 +1061,23 @@
         <v>0.12945100000000001</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="4">
-        <v>1.5483</v>
+        <v>1.5851</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1102,10 +1105,10 @@
         <v>5.0118999999999997E-2</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1127,7 +1130,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="15">
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1135,13 +1138,13 @@
         <v>19</v>
       </c>
       <c r="C7" s="1">
-        <v>2.8936000000000002</v>
+        <v>1.4815499999999999</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>16</v>
@@ -1159,21 +1162,21 @@
         <v>7.8569999999999994E-3</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="1">
-        <v>1.9992000000000001</v>
+        <v>1.3889</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>17</v>
@@ -1191,21 +1194,21 @@
         <v>2.9491E-2</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="1">
-        <v>1.8539000000000001</v>
+        <v>1.7917000000000001</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>29</v>
@@ -1223,10 +1226,10 @@
         <v>2.2523999999999999E-2</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1247,27 +1250,27 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" ht="15">
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="1">
-        <v>5.3746210000000003</v>
+        <v>1.5340499999999999</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>16</v>
@@ -1285,27 +1288,27 @@
         <v>5.7054000000000001E-2</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="1">
-        <v>2.204396</v>
+        <v>1.9049739999999999</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>17</v>
@@ -1323,27 +1326,27 @@
         <v>0.19664400000000001</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="1">
-        <v>2.9742760000000001</v>
+        <v>1.876174</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>29</v>
@@ -1361,10 +1364,10 @@
         <v>0.25310199999999999</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1385,21 +1388,21 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:20" ht="15">
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="1">
-        <v>2.7888899999999999</v>
+        <v>1.92988</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>14</v>
@@ -1408,10 +1411,10 @@
         <v>14</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
@@ -1428,24 +1431,24 @@
         <v>0.13206999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="1">
-        <v>2.0005999999999999</v>
+        <v>1.6651400000000001</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -1462,24 +1465,24 @@
         <v>6.5002000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="1">
-        <v>2.7941799999999999</v>
+        <v>1.8469</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -1496,27 +1499,27 @@
         <v>0.13918</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15">
+    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="1">
-        <v>4.9928999999999997</v>
+        <v>1.9643999999999999</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
@@ -1533,7 +1536,7 @@
         <v>8.3160000000000005E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1554,33 +1557,33 @@
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
     </row>
-    <row r="20" spans="1:20" ht="15">
+    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
@@ -1597,27 +1600,27 @@
         <v>2.1878999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
@@ -1634,27 +1637,27 @@
         <v>1.0095E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
@@ -1671,30 +1674,30 @@
         <v>5.6469999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -1711,7 +1714,7 @@
         <v>1.0437999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1732,33 +1735,33 @@
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
     </row>
-    <row r="25" spans="1:20" ht="15">
+    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1">
         <v>2.9815</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="O25" s="1">
         <v>1.039E-3</v>
@@ -1776,41 +1779,41 @@
         <v>4.6030000000000003E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1">
         <v>2.8500999999999999</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="15">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all done but just veocity
</commit_message>
<xml_diff>
--- a/FinalResults/trajectoryOpt.xlsx
+++ b/FinalResults/trajectoryOpt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koray\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koray_0\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5208067-418C-4F25-A745-2AAEA91B8BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965CDB43-3318-45B4-9C14-C3C1BB7C9D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
+    <workbookView xWindow="28680" yWindow="15" windowWidth="20730" windowHeight="11040" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
   <si>
     <t>Single Target - Single Section</t>
   </si>
@@ -208,63 +208,18 @@
     <t>0, 0.04, 0.03</t>
   </si>
   <si>
-    <t>0.46401      3.7851      4.9514</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.2448      7.5379      6.6401</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0734      8.3757      6.2183 </t>
-  </si>
-  <si>
-    <t>7.2343      6.6412      8.1195</t>
-  </si>
-  <si>
-    <t>0.59829      2.9572      4.3273</t>
-  </si>
-  <si>
-    <t>4.1828      1.4902      2.0095</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7.2786      6.4874     0.68338</t>
-  </si>
-  <si>
-    <t>7.5517       4.193      4.7719</t>
-  </si>
-  <si>
     <t>data17</t>
   </si>
   <si>
     <t>Line</t>
   </si>
   <si>
-    <t>0.77086      2.1752      2.6693</t>
-  </si>
-  <si>
-    <t>4.5301      3.5049      1.7147</t>
-  </si>
-  <si>
-    <t>4.5301      4.8938      3.9061</t>
-  </si>
-  <si>
-    <t>4.5301      4.5568      4.0878</t>
-  </si>
-  <si>
     <t>data18</t>
   </si>
   <si>
-    <t>0    0.0150    0.0100</t>
-  </si>
-  <si>
-    <t>0    0.0250    0.0300</t>
-  </si>
-  <si>
     <t>Target Point3</t>
   </si>
   <si>
-    <t>0    0.0350    0.0450</t>
-  </si>
-  <si>
     <t>CtrlPnt</t>
   </si>
   <si>
@@ -283,36 +238,9 @@
     <t>DoubleTargetSharp_NoKpKdZeta_3 Section</t>
   </si>
   <si>
-    <t>2.0662      2.6046      2.2889</t>
-  </si>
-  <si>
-    <t>2.2377      1.9964           4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0    0.029524    0.010001</t>
-  </si>
-  <si>
     <t>0    0.0450    0.0350</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2.1401      1.2805        2.05</t>
-  </si>
-  <si>
-    <t>2.2463       3.861      2.0857</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0       0.045    0.017914</t>
-  </si>
-  <si>
-    <t>Velocity(t_Vmax) one control point</t>
-  </si>
-  <si>
-    <t>Velocity(t_Vmax) two control point</t>
-  </si>
-  <si>
-    <t>data20</t>
-  </si>
-  <si>
     <t>14.9847           15      3.01046</t>
   </si>
   <si>
@@ -403,16 +331,109 @@
     <t>1.066      2.1154      1.3248</t>
   </si>
   <si>
-    <t xml:space="preserve">0.45319      1.3363      2.8087 </t>
-  </si>
-  <si>
-    <t>5.0797      2.8558      1.5681</t>
-  </si>
-  <si>
-    <t>5.0797      1.6178      6.7134</t>
-  </si>
-  <si>
-    <t>5.0797      5.2114      4.2905</t>
+    <t>0.4863      2.0044      3.2198</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.1706      2.8737        1.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.1706      2.1409      9.9744</t>
+  </si>
+  <si>
+    <t>5.1706      4.6206      4.5611</t>
+  </si>
+  <si>
+    <t>0.5233      1.1452      1.9808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0691      1.4385      2.0797  </t>
+  </si>
+  <si>
+    <t>3.3703      4.9853      1.1561</t>
+  </si>
+  <si>
+    <t>2.1466      2.9449           5</t>
+  </si>
+  <si>
+    <t>0.43433      1.1601      1.9963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.7961       3.609      3.0573 </t>
+  </si>
+  <si>
+    <t>3.3815       1.925      3.3221</t>
+  </si>
+  <si>
+    <t>2.4183      1.6134      3.9184</t>
+  </si>
+  <si>
+    <t>0.48116     0.94818       1.935</t>
+  </si>
+  <si>
+    <t>3.5276      2.7586      1.4303</t>
+  </si>
+  <si>
+    <t>1.5396      4.7235      2.4842</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.6288      2.3665      4.9999</t>
+  </si>
+  <si>
+    <t>Hyper Two Target Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.4914      4.6608</t>
+  </si>
+  <si>
+    <t>9.7524      5.0223</t>
+  </si>
+  <si>
+    <t>4.8855      5.7357</t>
+  </si>
+  <si>
+    <t>0, 0.015, 0.005</t>
+  </si>
+  <si>
+    <t>0, 0.035, 0.025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.014382   0.0045277   --- 0.035209    0.028134</t>
+  </si>
+  <si>
+    <t>Hyper Two Target Ordered</t>
+  </si>
+  <si>
+    <t>8.3619      7.1018</t>
+  </si>
+  <si>
+    <t>13.4095      9.14273</t>
+  </si>
+  <si>
+    <t>5.3061      9.9842</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.043146    0.032442  ----- 0.013443  -0.0084191</t>
+  </si>
+  <si>
+    <t>Hyper Five Target Ordered</t>
+  </si>
+  <si>
+    <t>data21</t>
+  </si>
+  <si>
+    <t>3.36968      11.2323</t>
+  </si>
+  <si>
+    <t>8.93463      11.5274</t>
+  </si>
+  <si>
+    <t>4.11346      11.5311</t>
+  </si>
+  <si>
+    <t>0.04883     0.02226  ----  0.010749  -0.0081906</t>
+  </si>
+  <si>
+    <t>0, 0.01, 0.02    --- 0, 0.035, 0.025 --- 0, 0.03, 0.01   ---0, 0.015, 0.005 ---0, 0.025, 0.04</t>
   </si>
 </sst>
 </file>
@@ -877,31 +898,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE33DE-026B-47FC-A290-185B7A79B5AD}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="30.375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="30.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.75" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.75" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.7109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="12" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.125" style="1"/>
+    <col min="19" max="19" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
@@ -912,7 +933,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -950,19 +971,19 @@
         <v>38</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>13</v>
@@ -974,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -989,7 +1010,7 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1020,7 +1041,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -1033,7 +1054,7 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -1077,7 +1098,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1108,7 +1129,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1130,7 +1151,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1141,10 +1162,10 @@
         <v>1.4815499999999999</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>16</v>
@@ -1165,7 +1186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1173,10 +1194,10 @@
         <v>1.3889</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>17</v>
@@ -1197,7 +1218,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1205,10 +1226,10 @@
         <v>1.7917000000000001</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>29</v>
@@ -1229,7 +1250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1250,7 +1271,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1261,16 +1282,16 @@
         <v>1.5340499999999999</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>16</v>
@@ -1291,7 +1312,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1299,16 +1320,16 @@
         <v>1.9049739999999999</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>17</v>
@@ -1329,7 +1350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1337,16 +1358,16 @@
         <v>1.876174</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>29</v>
@@ -1367,7 +1388,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1388,7 +1409,7 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -1399,10 +1420,10 @@
         <v>1.92988</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>14</v>
@@ -1431,7 +1452,7 @@
         <v>0.13206999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1439,16 +1460,16 @@
         <v>1.6651400000000001</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>39</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -1465,7 +1486,7 @@
         <v>6.5002000000000004E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1473,10 +1494,10 @@
         <v>1.8469</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>41</v>
@@ -1499,7 +1520,7 @@
         <v>0.13918</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -1510,10 +1531,10 @@
         <v>1.9643999999999999</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>34</v>
@@ -1536,7 +1557,7 @@
         <v>8.3160000000000005E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1557,27 +1578,27 @@
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
     </row>
-    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>34</v>
@@ -1600,21 +1621,21 @@
         <v>2.1878999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>39</v>
@@ -1637,21 +1658,21 @@
         <v>1.0095E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>41</v>
@@ -1674,24 +1695,24 @@
         <v>5.6469999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>34</v>
@@ -1714,7 +1735,7 @@
         <v>1.0437999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1735,33 +1756,33 @@
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
     </row>
-    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C25" s="1">
-        <v>2.9815</v>
+        <v>1.7575000000000001</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>71</v>
+        <v>112</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="O25" s="1">
         <v>1.039E-3</v>
@@ -1779,42 +1800,66 @@
         <v>4.6030000000000003E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>43</v>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C26" s="1">
-        <v>2.8500999999999999</v>
+        <v>1.556</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>69</v>
+        <v>119</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2.8978999999999999</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
14-17 DATA WILL BE FIGURED OUT
</commit_message>
<xml_diff>
--- a/FinalResults/trajectoryOpt.xlsx
+++ b/FinalResults/trajectoryOpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koray_0\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965CDB43-3318-45B4-9C14-C3C1BB7C9D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF841C3-B136-47C2-8FF0-9817E52C165F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="15" windowWidth="20730" windowHeight="11040" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
+    <workbookView xWindow="29970" yWindow="1305" windowWidth="15375" windowHeight="7785" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,9 +418,6 @@
     <t>Hyper Five Target Ordered</t>
   </si>
   <si>
-    <t>data21</t>
-  </si>
-  <si>
     <t>3.36968      11.2323</t>
   </si>
   <si>
@@ -434,6 +431,9 @@
   </si>
   <si>
     <t>0, 0.01, 0.02    --- 0, 0.035, 0.025 --- 0, 0.03, 0.01   ---0, 0.015, 0.005 ---0, 0.025, 0.04</t>
+  </si>
+  <si>
+    <t>data20</t>
   </si>
 </sst>
 </file>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE33DE-026B-47FC-A290-185B7A79B5AD}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,25 +1837,25 @@
         <v>122</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C27" s="1">
         <v>2.8978999999999999</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="K27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
data 14 keep going
</commit_message>
<xml_diff>
--- a/FinalResults/trajectoryOpt.xlsx
+++ b/FinalResults/trajectoryOpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koray\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7937B822-409C-4BEB-B00D-DC352E73569D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C171E30C-003C-43B9-BA2F-057DC3D2BB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26265" yWindow="2160" windowWidth="21600" windowHeight="11385" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
+    <workbookView xWindow="6090" yWindow="2535" windowWidth="21600" windowHeight="11385" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,18 +331,6 @@
     <t>1.066      2.1154      1.3248</t>
   </si>
   <si>
-    <t>0.4863      2.0044      3.2198</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.1706      2.8737        1.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.1706      2.1409      9.9744</t>
-  </si>
-  <si>
-    <t>5.1706      4.6206      4.5611</t>
-  </si>
-  <si>
     <t>0.5233      1.1452      1.9808</t>
   </si>
   <si>
@@ -434,6 +422,18 @@
   </si>
   <si>
     <t>0.044532     0.03058  -----  0.0065839  -0.0075095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.41893      1.07829      1.75187  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.64284      3.84032      1.95855  </t>
+  </si>
+  <si>
+    <t>3.64284      6.60227      27.4749</t>
+  </si>
+  <si>
+    <t>3.64284      29.8433      6.50145</t>
   </si>
 </sst>
 </file>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE33DE-026B-47FC-A290-185B7A79B5AD}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,19 +1586,19 @@
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>34</v>
@@ -1626,16 +1626,16 @@
         <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>39</v>
@@ -1663,16 +1663,16 @@
         <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>41</v>
@@ -1703,16 +1703,16 @@
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>34</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>55</v>
@@ -1767,22 +1767,22 @@
         <v>1.7575000000000001</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="O25" s="1">
         <v>1.039E-3</v>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>61</v>
@@ -1811,51 +1811,51 @@
         <v>2.0760000000000001</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>63</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C27" s="1">
         <v>2.8978999999999999</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="N27" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
all experiment is done
</commit_message>
<xml_diff>
--- a/FinalResults/trajectoryOpt.xlsx
+++ b/FinalResults/trajectoryOpt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koray\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koray_0\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C171E30C-003C-43B9-BA2F-057DC3D2BB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65E066-967A-4B23-B009-6375A53777AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="2535" windowWidth="21600" windowHeight="11385" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
+    <workbookView xWindow="29970" yWindow="1305" windowWidth="15375" windowHeight="7785" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,42 +331,6 @@
     <t>1.066      2.1154      1.3248</t>
   </si>
   <si>
-    <t>0.5233      1.1452      1.9808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0691      1.4385      2.0797  </t>
-  </si>
-  <si>
-    <t>3.3703      4.9853      1.1561</t>
-  </si>
-  <si>
-    <t>2.1466      2.9449           5</t>
-  </si>
-  <si>
-    <t>0.43433      1.1601      1.9963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.7961       3.609      3.0573 </t>
-  </si>
-  <si>
-    <t>3.3815       1.925      3.3221</t>
-  </si>
-  <si>
-    <t>2.4183      1.6134      3.9184</t>
-  </si>
-  <si>
-    <t>0.48116     0.94818       1.935</t>
-  </si>
-  <si>
-    <t>3.5276      2.7586      1.4303</t>
-  </si>
-  <si>
-    <t>1.5396      4.7235      2.4842</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.6288      2.3665      4.9999</t>
-  </si>
-  <si>
     <t>Hyper Two Target Line</t>
   </si>
   <si>
@@ -424,16 +388,52 @@
     <t>0.044532     0.03058  -----  0.0065839  -0.0075095</t>
   </si>
   <si>
-    <t xml:space="preserve">0.41893      1.07829      1.75187  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.64284      3.84032      1.95855  </t>
-  </si>
-  <si>
-    <t>3.64284      6.60227      27.4749</t>
-  </si>
-  <si>
-    <t>3.64284      29.8433      6.50145</t>
+    <t>0.576192     0.895692      1.73493</t>
+  </si>
+  <si>
+    <t>4.49918       3.0787      1.57671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.49918      1.50777      29.3524 </t>
+  </si>
+  <si>
+    <t>4.49918       5.8954      2.68569</t>
+  </si>
+  <si>
+    <t>0.242992      1.77835      1.79007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1      3.32578      5.12966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1       19.658      3.07353 </t>
+  </si>
+  <si>
+    <t>1      18.8954      25.8191</t>
+  </si>
+  <si>
+    <t>0.432502     0.966013       1.5413</t>
+  </si>
+  <si>
+    <t>1       15.185      13.2658</t>
+  </si>
+  <si>
+    <t>1       11.431      25.6703</t>
+  </si>
+  <si>
+    <t>1       7.3239      9.16861</t>
+  </si>
+  <si>
+    <t>0.51225      1.2425      1.9047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1      5.6425       2.886 </t>
+  </si>
+  <si>
+    <t>1      3.6187      4.8392</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1      3.1022      2.6144</t>
   </si>
 </sst>
 </file>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE33DE-026B-47FC-A290-185B7A79B5AD}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,19 +1586,19 @@
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>34</v>
@@ -1626,16 +1626,16 @@
         <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>39</v>
@@ -1663,16 +1663,16 @@
         <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>41</v>
@@ -1703,16 +1703,16 @@
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>34</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>55</v>
@@ -1767,22 +1767,22 @@
         <v>1.7575000000000001</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="O25" s="1">
         <v>1.039E-3</v>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>61</v>
@@ -1811,51 +1811,51 @@
         <v>2.0760000000000001</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>63</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C27" s="1">
         <v>2.8978999999999999</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gain data almost done
</commit_message>
<xml_diff>
--- a/FinalResults/trajectoryOpt.xlsx
+++ b/FinalResults/trajectoryOpt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koray_0\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koray\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65E066-967A-4B23-B009-6375A53777AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BB323B-3163-4032-8060-0BDA90F6424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="1305" windowWidth="15375" windowHeight="7785" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -898,19 +898,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE33DE-026B-47FC-A290-185B7A79B5AD}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="30.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="17.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="20.7109375" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
all plots is done
</commit_message>
<xml_diff>
--- a/FinalResults/trajectoryOpt.xlsx
+++ b/FinalResults/trajectoryOpt.xlsx
@@ -2,34 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koray\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koray_0\Documents\GitHub\Trajectory_Optimization\FinalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BB323B-3163-4032-8060-0BDA90F6424E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467142BB-6C44-431C-9842-013B560E3315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
+    <workbookView xWindow="28680" yWindow="15" windowWidth="20730" windowHeight="11040" tabRatio="201" xr2:uid="{E435F10A-0C78-41AE-9AD4-61BD5C4634DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -898,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE33DE-026B-47FC-A290-185B7A79B5AD}">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +904,8 @@
     <col min="9" max="9" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="13.7109375" style="1" customWidth="1"/>

</xml_diff>